<commit_message>
Finish off CountIfs demo
</commit_message>
<xml_diff>
--- a/Basic Analysis/Conditional Aggregations/Multiple conditions - Countifs Sumifs.xlsx
+++ b/Basic Analysis/Conditional Aggregations/Multiple conditions - Countifs Sumifs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sites\Data_Foundations_WithYouWithMe\Basic Analysis\Conditional Aggregations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC84236-4A35-4A6B-AF52-1A92C29624A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37F8A93-357A-46CC-82A1-50FD9EDB9336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1395" windowWidth="29850" windowHeight="14805" firstSheet="1" activeTab="1" xr2:uid="{682ECE72-A850-4EEA-BAD4-BC6FFFC5916E}"/>
+    <workbookView xWindow="1560" yWindow="675" windowWidth="29850" windowHeight="14805" firstSheet="1" activeTab="1" xr2:uid="{682ECE72-A850-4EEA-BAD4-BC6FFFC5916E}"/>
   </bookViews>
   <sheets>
     <sheet name="Objectives" sheetId="3" r:id="rId1"/>
@@ -3391,6 +3391,24 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3435,24 +3453,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4044,7 +4044,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
+      <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4114,23 +4114,23 @@
       <c r="G2" s="13">
         <v>7.25</v>
       </c>
-      <c r="J2" s="62" t="s">
+      <c r="J2" s="47" t="s">
         <v>924</v>
       </c>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="R2" s="62" t="s">
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="R2" s="47" t="s">
         <v>925</v>
       </c>
-      <c r="S2" s="62"/>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62"/>
-      <c r="V2" s="62"/>
-      <c r="W2" s="62"/>
-      <c r="X2" s="62"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
+      <c r="V2" s="47"/>
+      <c r="W2" s="47"/>
+      <c r="X2" s="47"/>
       <c r="Y2" s="18"/>
       <c r="Z2" s="18"/>
     </row>
@@ -4156,27 +4156,27 @@
       <c r="G3" s="13">
         <v>71.283299999999997</v>
       </c>
-      <c r="J3" s="61" t="s">
+      <c r="J3" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="63" t="s">
+      <c r="K3" s="48" t="s">
         <v>940</v>
       </c>
-      <c r="L3" s="63"/>
-      <c r="M3" s="63"/>
-      <c r="N3" s="63"/>
-      <c r="O3" s="64"/>
-      <c r="R3" s="61" t="s">
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="49"/>
+      <c r="R3" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="S3" s="63" t="s">
+      <c r="S3" s="48" t="s">
         <v>926</v>
       </c>
-      <c r="T3" s="63"/>
-      <c r="U3" s="63"/>
-      <c r="V3" s="63"/>
-      <c r="W3" s="63"/>
-      <c r="X3" s="64"/>
+      <c r="T3" s="48"/>
+      <c r="U3" s="48"/>
+      <c r="V3" s="48"/>
+      <c r="W3" s="48"/>
+      <c r="X3" s="49"/>
       <c r="Y3" s="18"/>
       <c r="Z3" s="18"/>
     </row>
@@ -4202,19 +4202,19 @@
       <c r="G4" s="13">
         <v>7.9249999999999998</v>
       </c>
-      <c r="J4" s="61"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="65"/>
-      <c r="M4" s="65"/>
-      <c r="N4" s="65"/>
-      <c r="O4" s="66"/>
-      <c r="R4" s="61"/>
-      <c r="S4" s="65"/>
-      <c r="T4" s="65"/>
-      <c r="U4" s="65"/>
-      <c r="V4" s="65"/>
-      <c r="W4" s="65"/>
-      <c r="X4" s="66"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="M4" s="50"/>
+      <c r="N4" s="50"/>
+      <c r="O4" s="51"/>
+      <c r="R4" s="46"/>
+      <c r="S4" s="50"/>
+      <c r="T4" s="50"/>
+      <c r="U4" s="50"/>
+      <c r="V4" s="50"/>
+      <c r="W4" s="50"/>
+      <c r="X4" s="51"/>
       <c r="Y4" s="18"/>
       <c r="Z4" s="18"/>
     </row>
@@ -4240,27 +4240,27 @@
       <c r="G5" s="13">
         <v>53.1</v>
       </c>
-      <c r="J5" s="59" t="s">
+      <c r="J5" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="46" t="s">
+      <c r="K5" s="52" t="s">
         <v>927</v>
       </c>
-      <c r="L5" s="46"/>
-      <c r="M5" s="46"/>
-      <c r="N5" s="46"/>
-      <c r="O5" s="46"/>
-      <c r="R5" s="59" t="s">
+      <c r="L5" s="52"/>
+      <c r="M5" s="52"/>
+      <c r="N5" s="52"/>
+      <c r="O5" s="52"/>
+      <c r="R5" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="S5" s="46" t="s">
+      <c r="S5" s="52" t="s">
         <v>949</v>
       </c>
-      <c r="T5" s="46"/>
-      <c r="U5" s="46"/>
-      <c r="V5" s="46"/>
-      <c r="W5" s="46"/>
-      <c r="X5" s="46"/>
+      <c r="T5" s="52"/>
+      <c r="U5" s="52"/>
+      <c r="V5" s="52"/>
+      <c r="W5" s="52"/>
+      <c r="X5" s="52"/>
       <c r="Y5" s="18"/>
       <c r="Z5" s="18"/>
     </row>
@@ -4286,19 +4286,19 @@
       <c r="G6" s="13">
         <v>8.0500000000000007</v>
       </c>
-      <c r="J6" s="60"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="46"/>
-      <c r="O6" s="46"/>
-      <c r="R6" s="60"/>
-      <c r="S6" s="46"/>
-      <c r="T6" s="46"/>
-      <c r="U6" s="46"/>
-      <c r="V6" s="46"/>
-      <c r="W6" s="46"/>
-      <c r="X6" s="46"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="52"/>
+      <c r="N6" s="52"/>
+      <c r="O6" s="52"/>
+      <c r="R6" s="66"/>
+      <c r="S6" s="52"/>
+      <c r="T6" s="52"/>
+      <c r="U6" s="52"/>
+      <c r="V6" s="52"/>
+      <c r="W6" s="52"/>
+      <c r="X6" s="52"/>
       <c r="Y6" s="18"/>
       <c r="Z6" s="18"/>
     </row>
@@ -4347,19 +4347,19 @@
       <c r="G8" s="13">
         <v>51.862499999999997</v>
       </c>
-      <c r="J8" s="55" t="s">
+      <c r="J8" s="61" t="s">
         <v>941</v>
       </c>
-      <c r="K8" s="55"/>
+      <c r="K8" s="61"/>
       <c r="L8" s="9">
         <f>COUNTIFS(E:E,"male",C:C,"First")</f>
         <v>122</v>
       </c>
-      <c r="R8" s="56" t="s">
+      <c r="R8" s="62" t="s">
         <v>946</v>
       </c>
-      <c r="S8" s="57"/>
-      <c r="T8" s="58"/>
+      <c r="S8" s="63"/>
+      <c r="T8" s="64"/>
       <c r="U8" s="16"/>
     </row>
     <row r="9" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -4436,31 +4436,31 @@
       <c r="G11" s="13">
         <v>30.070799999999998</v>
       </c>
-      <c r="J11" s="51" t="s">
+      <c r="J11" s="57" t="s">
         <v>931</v>
       </c>
-      <c r="K11" s="47" t="s">
+      <c r="K11" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="L11" s="48"/>
-      <c r="M11" s="49" t="s">
+      <c r="L11" s="54"/>
+      <c r="M11" s="55" t="s">
         <v>933</v>
       </c>
       <c r="R11" s="23" t="s">
         <v>935</v>
       </c>
-      <c r="S11" s="53" t="s">
+      <c r="S11" s="59" t="s">
         <v>936</v>
       </c>
-      <c r="T11" s="54"/>
-      <c r="U11" s="53" t="s">
+      <c r="T11" s="60"/>
+      <c r="U11" s="59" t="s">
         <v>937</v>
       </c>
-      <c r="V11" s="54"/>
-      <c r="W11" s="53" t="s">
+      <c r="V11" s="60"/>
+      <c r="W11" s="59" t="s">
         <v>938</v>
       </c>
-      <c r="X11" s="54"/>
+      <c r="X11" s="60"/>
     </row>
     <row r="12" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
@@ -4484,14 +4484,14 @@
       <c r="G12" s="13">
         <v>16.7</v>
       </c>
-      <c r="J12" s="52"/>
+      <c r="J12" s="58"/>
       <c r="K12" s="10" t="s">
         <v>929</v>
       </c>
       <c r="L12" s="10" t="s">
         <v>932</v>
       </c>
-      <c r="M12" s="50"/>
+      <c r="M12" s="56"/>
       <c r="R12" s="24"/>
       <c r="S12" s="10" t="s">
         <v>31</v>
@@ -4537,9 +4537,18 @@
       <c r="J13" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="11"/>
+      <c r="K13" s="9">
+        <f>COUNTIFS($C:$C,J13,$B:$B,"Yes")</f>
+        <v>136</v>
+      </c>
+      <c r="L13" s="9">
+        <f>COUNTIFS($C:$C,J13,$B:$B,"No")</f>
+        <v>80</v>
+      </c>
+      <c r="M13" s="11">
+        <f>K13/(K13+L13)</f>
+        <v>0.62962962962962965</v>
+      </c>
       <c r="P13" s="5"/>
       <c r="R13" s="19" t="s">
         <v>32</v>
@@ -4576,9 +4585,18 @@
       <c r="J14" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="11"/>
+      <c r="K14" s="9">
+        <f t="shared" ref="K14:K15" si="0">COUNTIFS($C:$C,J14,$B:$B,"Yes")</f>
+        <v>87</v>
+      </c>
+      <c r="L14" s="9">
+        <f t="shared" ref="L14:L15" si="1">COUNTIFS($C:$C,J14,$B:$B,"No")</f>
+        <v>97</v>
+      </c>
+      <c r="M14" s="11">
+        <f t="shared" ref="M14:M16" si="2">K14/(K14+L14)</f>
+        <v>0.47282608695652173</v>
+      </c>
       <c r="P14" s="5"/>
       <c r="R14" s="19" t="s">
         <v>42</v>
@@ -4615,9 +4633,18 @@
       <c r="J15" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="11"/>
+      <c r="K15" s="9">
+        <f t="shared" si="0"/>
+        <v>119</v>
+      </c>
+      <c r="L15" s="9">
+        <f t="shared" si="1"/>
+        <v>368</v>
+      </c>
+      <c r="M15" s="11">
+        <f t="shared" si="2"/>
+        <v>0.24435318275154005</v>
+      </c>
       <c r="R15" s="19" t="s">
         <v>29</v>
       </c>
@@ -4653,9 +4680,18 @@
       <c r="J16" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="11"/>
+      <c r="K16" s="9">
+        <f>SUM(K13:K15)</f>
+        <v>342</v>
+      </c>
+      <c r="L16" s="9">
+        <f>SUM(L13:L15)</f>
+        <v>545</v>
+      </c>
+      <c r="M16" s="11">
+        <f t="shared" si="2"/>
+        <v>0.38556933483652761</v>
+      </c>
       <c r="R16" s="20" t="s">
         <v>19</v>
       </c>
@@ -24730,12 +24766,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="J2:O2"/>
-    <mergeCell ref="R2:X2"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:O4"/>
-    <mergeCell ref="S3:X4"/>
     <mergeCell ref="K5:O6"/>
     <mergeCell ref="S5:X6"/>
     <mergeCell ref="K11:L11"/>
@@ -24748,6 +24778,12 @@
     <mergeCell ref="R8:T8"/>
     <mergeCell ref="R5:R6"/>
     <mergeCell ref="J5:J6"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="J2:O2"/>
+    <mergeCell ref="R2:X2"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:O4"/>
+    <mergeCell ref="S3:X4"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>